<commit_message>
feat: finish basic database table design
</commit_message>
<xml_diff>
--- a/ustc_printer_sql.xlsx
+++ b/ustc_printer_sql.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10435\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaohan4\Desktop\ustc_printer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C48E01-BC89-49F1-8B57-43DF3B27DAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2350" yWindow="3920" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2350" yWindow="3920" windowWidth="28800" windowHeight="15370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,16 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>订单表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>打印文件名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -67,22 +62,298 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>订单id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除标志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（匿名用户， 管理员，超级管理员)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户-订单 一对多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色-用户 一对多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色-权限 多对多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除标志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地址表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地址id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>校区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公寓号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>寝室号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>订单id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单价格</t>
+    <t>角色-权限表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户-地址： 1:N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配送地址（与地址表无太大关联)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>营收表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>营收id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>print_color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paper_size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delivery_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>others</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超时重发邮件（也给我发一个)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delivery_address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apartment_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dormitory_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phone_number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>others</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_perm_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perm_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>revenue_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定时任务创建</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,82 +390,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -211,10 +417,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="2D3236"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -468,69 +674,339 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.58203125" customWidth="1"/>
+    <col min="7" max="7" width="14.25" customWidth="1"/>
+    <col min="8" max="8" width="12.58203125" customWidth="1"/>
+    <col min="11" max="11" width="9.58203125" customWidth="1"/>
+    <col min="12" max="12" width="11.08203125" customWidth="1"/>
+    <col min="13" max="13" width="27.08203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sql table, POJO and basic mapper
</commit_message>
<xml_diff>
--- a/ustc_printer_sql.xlsx
+++ b/ustc_printer_sql.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaohan4\Desktop\ustc_printer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10435\IdeaProjects\ustc_printer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0019CE0-278A-495A-A380-A67C6FDBBFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2350" yWindow="3920" windowWidth="28800" windowHeight="15370"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="18500" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>订单表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,10 +187,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>营收表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>营收id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -218,91 +215,103 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>paper_size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>delivery_mode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超时重发邮件（也给我发一个)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delivery_address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apartment_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dormitory_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>phone_number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>others</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is_delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>订单状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>超时重发邮件（也给我发一个)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delivery_address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update_time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>qq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>role_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>创建日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>address_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apartment_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dormitory_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phone_number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>others</t>
+    <t>role_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role_perm_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -310,26 +319,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>role_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>permission_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>permission_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role_perm_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>role_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>perm_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -347,13 +336,81 @@
   </si>
   <si>
     <t>定时任务创建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流水表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑白页数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>彩色页数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A3数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A4数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A5数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>照片数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>价目表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>价格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(a3,a4,黑白彩色等等)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page_numbers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（不用，订单表中已经包含)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page_size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>other_demand</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -674,11 +731,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -694,12 +751,12 @@
     <col min="13" max="13" width="27.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -716,87 +773,93 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
         <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>51</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="L3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="41" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="41" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H4" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="28" x14ac:dyDescent="0.3">
       <c r="L5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -816,30 +879,30 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -847,7 +910,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -870,36 +933,36 @@
         <v>37</v>
       </c>
       <c r="H11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" t="s">
-        <v>69</v>
-      </c>
       <c r="H12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -907,7 +970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -918,20 +981,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -939,20 +1002,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -963,45 +1026,90 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>74</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
         <v>75</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" t="s">
-        <v>79</v>
+    <row r="31" spans="1:9" s="1" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>